<commit_message>
P2p implementation changes and completed status
</commit_message>
<xml_diff>
--- a/src/main/java/dataRepository/logindata.xlsx
+++ b/src/main/java/dataRepository/logindata.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t xml:space="preserve">UserName</t>
   </si>
@@ -28,13 +28,46 @@
     <t xml:space="preserve">Password</t>
   </si>
   <si>
-    <t xml:space="preserve">exu51@mailinator.com</t>
+    <t xml:space="preserve">Auttesttt_4@mailinator.com</t>
   </si>
   <si>
     <t xml:space="preserve">password</t>
   </si>
   <si>
-    <t xml:space="preserve">exu52@mailinator.com</t>
+    <t xml:space="preserve">Auttesttt_5@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auttesttt_6@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auttesttt_7@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auttesttt_8@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auttesttt_9@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auttesttt_10@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auttesttt_11@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auttesttt_12@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auttesttt_13@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auttesttt_14@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auttesttt_15@mailinator.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auttesttt_16@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -142,20 +175,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="1" hidden="false" style="0" width="24.3010204081633" collapsed="true"/>
-    <col min="2" max="2" hidden="false" style="0" width="10.9336734693878" collapsed="true"/>
-    <col min="3" max="7" hidden="false" style="0" width="8.36734693877551" collapsed="true"/>
-    <col min="8" max="8" hidden="false" style="0" width="30.5102040816327" collapsed="true"/>
-    <col min="9" max="9" hidden="false" style="0" width="22.6785714285714" collapsed="true"/>
-    <col min="10" max="1025" hidden="false" style="0" width="8.36734693877551" collapsed="true"/>
+    <col min="1" max="1" hidden="false" style="0" width="23.0816326530612" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="10.530612244898" collapsed="true"/>
+    <col min="3" max="7" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="29.4285714285714" collapsed="true"/>
+    <col min="9" max="9" hidden="false" style="0" width="21.8673469387755" collapsed="true"/>
+    <col min="10" max="1025" hidden="false" style="0" width="8.50510204081633" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -167,18 +200,62 @@
       </c>
     </row>
     <row r="2" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
+      <c r="A2" s="0" t="s">
+        <v>9</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="3" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="exu51@mailinator.com"/>
-    <hyperlink ref="A3" r:id="rId2" display="exu52@mailinator.com"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
changed xpath for feedback thank u page
</commit_message>
<xml_diff>
--- a/src/main/java/dataRepository/logindata.xlsx
+++ b/src/main/java/dataRepository/logindata.xlsx
@@ -324,7 +324,7 @@
     </row>
     <row r="2" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>3</v>
@@ -332,7 +332,7 @@
     </row>
     <row r="3" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>3</v>
@@ -340,7 +340,7 @@
     </row>
     <row r="4" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>3</v>
@@ -348,7 +348,7 @@
     </row>
     <row r="5" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>3</v>
@@ -356,7 +356,7 @@
     </row>
     <row r="6" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>3</v>
@@ -364,7 +364,7 @@
     </row>
     <row r="7" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>3</v>
@@ -372,7 +372,7 @@
     </row>
     <row r="8" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>3</v>
@@ -380,7 +380,7 @@
     </row>
     <row r="9" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>3</v>
@@ -388,7 +388,7 @@
     </row>
     <row r="10" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>3</v>
@@ -396,7 +396,7 @@
     </row>
     <row r="11" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>3</v>
@@ -404,7 +404,7 @@
     </row>
     <row r="12" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>3</v>
@@ -412,7 +412,7 @@
     </row>
     <row r="13" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>3</v>
@@ -420,7 +420,7 @@
     </row>
     <row r="14" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>3</v>
@@ -428,7 +428,7 @@
     </row>
     <row r="15" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>3</v>
@@ -436,7 +436,7 @@
     </row>
     <row r="16" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>3</v>
@@ -444,7 +444,7 @@
     </row>
     <row r="17" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>3</v>
@@ -452,7 +452,7 @@
     </row>
     <row r="18" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>3</v>
@@ -460,7 +460,7 @@
     </row>
     <row r="19" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>3</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="20" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>3</v>
@@ -476,7 +476,7 @@
     </row>
     <row r="21" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>3</v>
@@ -484,7 +484,7 @@
     </row>
     <row r="22" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>3</v>
@@ -492,7 +492,7 @@
     </row>
     <row r="23" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>3</v>
@@ -500,7 +500,7 @@
     </row>
     <row r="24" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>3</v>
@@ -508,7 +508,7 @@
     </row>
     <row r="25" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>3</v>
@@ -516,7 +516,7 @@
     </row>
     <row r="26" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>3</v>
@@ -524,7 +524,7 @@
     </row>
     <row r="27" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>3</v>
@@ -532,7 +532,7 @@
     </row>
     <row r="28" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>3</v>
@@ -540,7 +540,7 @@
     </row>
     <row r="29" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>3</v>
@@ -548,7 +548,7 @@
     </row>
     <row r="30" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>3</v>
@@ -556,7 +556,7 @@
     </row>
     <row r="31" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>3</v>
@@ -564,7 +564,7 @@
     </row>
     <row r="32" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>3</v>
@@ -572,7 +572,7 @@
     </row>
     <row r="33" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>3</v>
@@ -580,7 +580,7 @@
     </row>
     <row r="34" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>3</v>
@@ -588,7 +588,7 @@
     </row>
     <row r="35" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>3</v>
@@ -596,7 +596,7 @@
     </row>
     <row r="36" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>3</v>
@@ -604,7 +604,7 @@
     </row>
     <row r="37" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>3</v>
@@ -612,7 +612,7 @@
     </row>
     <row r="38" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>3</v>
@@ -620,7 +620,7 @@
     </row>
     <row r="39" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>3</v>
@@ -628,7 +628,7 @@
     </row>
     <row r="40" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>3</v>
@@ -636,7 +636,7 @@
     </row>
     <row r="41" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>3</v>
@@ -644,7 +644,7 @@
     </row>
     <row r="42" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>3</v>
@@ -652,7 +652,7 @@
     </row>
     <row r="43" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>3</v>
@@ -660,7 +660,7 @@
     </row>
     <row r="44" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>3</v>
@@ -668,7 +668,7 @@
     </row>
     <row r="45" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>3</v>
@@ -676,7 +676,7 @@
     </row>
     <row r="46" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>3</v>
@@ -684,7 +684,7 @@
     </row>
     <row r="47" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>3</v>
@@ -692,7 +692,7 @@
     </row>
     <row r="48" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B48" s="0" t="s">
         <v>3</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="49" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B49" s="0" t="s">
         <v>3</v>
@@ -708,7 +708,7 @@
     </row>
     <row r="50" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>3</v>
@@ -716,7 +716,7 @@
     </row>
     <row r="51" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>3</v>
@@ -724,25 +724,9 @@
     </row>
     <row r="52" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B53" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B54" s="0" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correction of jpurneypage reference
</commit_message>
<xml_diff>
--- a/src/main/java/dataRepository/logindata.xlsx
+++ b/src/main/java/dataRepository/logindata.xlsx
@@ -388,12 +388,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.8724489795918"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="7" min="3" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.0510204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.36734693877551"/>
+    <col min="1" max="1" hidden="false" style="0" width="35.8724489795918" collapsed="true"/>
+    <col min="2" max="2" hidden="false" style="0" width="9.31632653061224" collapsed="true"/>
+    <col min="3" max="7" hidden="false" style="0" width="8.36734693877551" collapsed="true"/>
+    <col min="8" max="8" hidden="false" style="0" width="26.0510204081633" collapsed="true"/>
+    <col min="9" max="9" hidden="false" style="0" width="19.3061224489796" collapsed="true"/>
+    <col min="10" max="1025" hidden="false" style="0" width="8.36734693877551" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -404,643 +404,619 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
+    <row r="3" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>7</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>5</v>
+    <row r="4" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>8</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
+    <row r="5" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>9</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B48" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B49" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B53" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B54" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B55" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B56" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B58" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B59" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B60" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B61" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B62" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B63" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B64" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B65" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B66" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B67" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B68" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B69" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B70" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B71" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B72" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B73" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B74" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B75" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B76" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B77" s="0" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="B79" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="B80" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="B81" s="0" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added thread to scorm quiz
</commit_message>
<xml_diff>
--- a/src/main/java/dataRepository/logindata.xlsx
+++ b/src/main/java/dataRepository/logindata.xlsx
@@ -337,7 +337,7 @@
     </row>
     <row r="2" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>3</v>
@@ -345,7 +345,7 @@
     </row>
     <row r="3" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>3</v>
@@ -353,7 +353,7 @@
     </row>
     <row r="4" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>3</v>
@@ -361,7 +361,7 @@
     </row>
     <row r="5" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>3</v>
@@ -369,7 +369,7 @@
     </row>
     <row r="6" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>3</v>
@@ -377,7 +377,7 @@
     </row>
     <row r="7" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>3</v>
@@ -385,7 +385,7 @@
     </row>
     <row r="8" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>3</v>
@@ -393,7 +393,7 @@
     </row>
     <row r="9" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>3</v>
@@ -401,7 +401,7 @@
     </row>
     <row r="10" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>3</v>
@@ -409,7 +409,7 @@
     </row>
     <row r="11" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>3</v>
@@ -417,7 +417,7 @@
     </row>
     <row r="12" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>3</v>
@@ -425,7 +425,7 @@
     </row>
     <row r="13" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>3</v>
@@ -433,7 +433,7 @@
     </row>
     <row r="14" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>3</v>
@@ -441,7 +441,7 @@
     </row>
     <row r="15" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>3</v>
@@ -449,7 +449,7 @@
     </row>
     <row r="16" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>3</v>
@@ -457,7 +457,7 @@
     </row>
     <row r="17" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>3</v>
@@ -465,7 +465,7 @@
     </row>
     <row r="18" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>3</v>
@@ -473,7 +473,7 @@
     </row>
     <row r="19" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>3</v>
@@ -481,7 +481,7 @@
     </row>
     <row r="20" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>3</v>
@@ -489,7 +489,7 @@
     </row>
     <row r="21" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>3</v>
@@ -497,7 +497,7 @@
     </row>
     <row r="22" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>3</v>
@@ -505,7 +505,7 @@
     </row>
     <row r="23" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>3</v>
@@ -513,7 +513,7 @@
     </row>
     <row r="24" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>3</v>
@@ -521,7 +521,7 @@
     </row>
     <row r="25" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>3</v>
@@ -529,7 +529,7 @@
     </row>
     <row r="26" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>3</v>
@@ -537,7 +537,7 @@
     </row>
     <row r="27" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>3</v>
@@ -545,7 +545,7 @@
     </row>
     <row r="28" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>3</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="29" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>3</v>
@@ -561,7 +561,7 @@
     </row>
     <row r="30" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B30" s="0" t="s">
         <v>3</v>
@@ -569,7 +569,7 @@
     </row>
     <row r="31" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B31" s="0" t="s">
         <v>3</v>
@@ -577,7 +577,7 @@
     </row>
     <row r="32" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B32" s="0" t="s">
         <v>3</v>
@@ -585,7 +585,7 @@
     </row>
     <row r="33" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>3</v>
@@ -593,7 +593,7 @@
     </row>
     <row r="34" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B34" s="0" t="s">
         <v>3</v>
@@ -601,7 +601,7 @@
     </row>
     <row r="35" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B35" s="0" t="s">
         <v>3</v>
@@ -609,7 +609,7 @@
     </row>
     <row r="36" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>3</v>
@@ -617,7 +617,7 @@
     </row>
     <row r="37" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B37" s="0" t="s">
         <v>3</v>
@@ -625,7 +625,7 @@
     </row>
     <row r="38" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B38" s="0" t="s">
         <v>3</v>
@@ -633,7 +633,7 @@
     </row>
     <row r="39" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="B39" s="0" t="s">
         <v>3</v>
@@ -641,7 +641,7 @@
     </row>
     <row r="40" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B40" s="0" t="s">
         <v>3</v>
@@ -649,7 +649,7 @@
     </row>
     <row r="41" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B41" s="0" t="s">
         <v>3</v>
@@ -657,7 +657,7 @@
     </row>
     <row r="42" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B42" s="0" t="s">
         <v>3</v>
@@ -665,7 +665,7 @@
     </row>
     <row r="43" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>3</v>
@@ -673,7 +673,7 @@
     </row>
     <row r="44" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="B44" s="0" t="s">
         <v>3</v>
@@ -681,7 +681,7 @@
     </row>
     <row r="45" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>3</v>
@@ -689,7 +689,7 @@
     </row>
     <row r="46" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="B46" s="0" t="s">
         <v>3</v>
@@ -697,7 +697,7 @@
     </row>
     <row r="47" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="B47" s="0" t="s">
         <v>3</v>
@@ -705,7 +705,7 @@
     </row>
     <row r="48" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B48" s="0" t="s">
         <v>3</v>
@@ -713,7 +713,7 @@
     </row>
     <row r="49" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B49" s="0" t="s">
         <v>3</v>
@@ -721,7 +721,7 @@
     </row>
     <row r="50" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>3</v>
@@ -729,7 +729,7 @@
     </row>
     <row r="51" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B51" s="0" t="s">
         <v>3</v>
@@ -737,7 +737,7 @@
     </row>
     <row r="52" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="B52" s="0" t="s">
         <v>3</v>
@@ -745,7 +745,7 @@
     </row>
     <row r="53" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B53" s="0" t="s">
         <v>3</v>
@@ -753,7 +753,7 @@
     </row>
     <row r="54" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B54" s="0" t="s">
         <v>3</v>
@@ -761,41 +761,9 @@
     </row>
     <row r="55" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="B56" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B57" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B58" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" hidden="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B59" s="0" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>